<commit_message>
some modifications in pipeline
</commit_message>
<xml_diff>
--- a/Playground/Evaluate_Answers/excel/grades.xlsx
+++ b/Playground/Evaluate_Answers/excel/grades.xlsx
@@ -1,33 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="grades" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="grades" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,80 +49,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -409,192 +350,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Q1</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Q2</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Q3</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Q4</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Q5</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Q6</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Q7</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Q8</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Q9</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Q10</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Q11</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Q12</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Q13</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Q14</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Q15</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Q16</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Q17</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>Q18</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Q19</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Q20</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1170517</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4</v>
-      </c>
-      <c r="F2" t="n">
-        <v>5</v>
-      </c>
-      <c r="G2" t="n">
-        <v>4</v>
-      </c>
-      <c r="H2" t="n">
-        <v>3</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>3</v>
-      </c>
-      <c r="K2" t="n">
-        <v>4</v>
-      </c>
-      <c r="L2" t="n">
-        <v>2</v>
-      </c>
-      <c r="M2" t="n">
-        <v>2</v>
-      </c>
-      <c r="N2" t="n">
-        <v>3</v>
-      </c>
-      <c r="O2" t="n">
-        <v>3</v>
-      </c>
-      <c r="P2" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>2</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
evalute answer + excel is done
</commit_message>
<xml_diff>
--- a/Playground/Evaluate_Answers/excel/grades.xlsx
+++ b/Playground/Evaluate_Answers/excel/grades.xlsx
@@ -1,36 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="grades" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="grades" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,18 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -350,15 +409,284 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S5" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Q5</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Q6</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Q7</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Q8</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Q9</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Q10</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Q11</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Q12</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Q13</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Q14</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Q15</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Q16</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Q17</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Q18</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Q19</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Q20</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Q21</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Q22</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>Q23</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>Q24</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>Q25</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>Q26</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>Q27</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>Q28</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>Q29</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>Grade:</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1170899</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>29.0/30</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>